<commit_message>
Bugs escollir grups, enviar mail arreglat
</commit_message>
<xml_diff>
--- a/excel_emplenat.xlsx
+++ b/excel_emplenat.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
   <si>
     <t>Grups</t>
   </si>
@@ -41,61 +41,61 @@
     <t>PADs Prof.</t>
   </si>
   <si>
-    <t>ampli p</t>
+    <t>ampli P</t>
   </si>
   <si>
-    <t>ampli t</t>
+    <t>ampli T</t>
   </si>
   <si>
-    <t>ampli elect p</t>
+    <t>ampli elect P</t>
   </si>
   <si>
-    <t>ampli elect t</t>
+    <t>ampli elect T</t>
   </si>
   <si>
-    <t>electronica p</t>
+    <t>electronica P</t>
   </si>
   <si>
-    <t>electronica t</t>
+    <t>electronica T</t>
   </si>
   <si>
-    <t>electrotecnia p</t>
+    <t>electrotecnia P</t>
   </si>
   <si>
-    <t>electrotecnia t</t>
+    <t>electrotecnia T</t>
   </si>
   <si>
-    <t>fluids p</t>
+    <t>fluids P</t>
   </si>
   <si>
-    <t>instrumentacio p</t>
+    <t>instrumentacio P</t>
   </si>
   <si>
-    <t>instrumentacio t</t>
+    <t>instrumentacio T</t>
   </si>
   <si>
-    <t>robot p</t>
+    <t>robot P</t>
   </si>
   <si>
-    <t>robot t</t>
+    <t>robot T</t>
   </si>
   <si>
-    <t>sistemes p</t>
+    <t>sistemes P</t>
   </si>
   <si>
-    <t>sistemes t</t>
+    <t>sistemes T</t>
   </si>
   <si>
-    <t>taller elèctric t</t>
+    <t>taller elèctric T</t>
   </si>
   <si>
-    <t>tallet elèctric p</t>
+    <t>tallet elèctric P</t>
   </si>
   <si>
-    <t>tfg t</t>
+    <t>tfg T</t>
   </si>
   <si>
-    <t>tfm t</t>
+    <t>tfm T</t>
   </si>
   <si>
     <t>LB</t>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>D5</t>
-  </si>
-  <si>
-    <t>profe</t>
   </si>
   <si>
     <t>Nom</t>
@@ -697,12 +694,12 @@
   <dimension ref="A1:AMK81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2:E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11.902834008097" customWidth="true" style="1"/>
+    <col min="1" max="1" width="12.210526315789" customWidth="true" style="1"/>
     <col min="2" max="2" width="7.497975708502" customWidth="true" style="1"/>
     <col min="3" max="3" width="6.5344129554656" customWidth="true" style="1"/>
     <col min="4" max="4" width="8.1417004048583" customWidth="true" style="1"/>
@@ -1735,7 +1732,7 @@
       </c>
       <c r="B1" s="3">
         <f>SUM(D1:BA1)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="5">
@@ -1760,7 +1757,7 @@
       </c>
       <c r="I1" s="5">
         <f>IF(I5="","",SUM(I6:I81))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J1" s="5">
         <f>IF(J5="","",SUM(J6:J81))</f>
@@ -2044,7 +2041,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="3">
         <f>SUM(D3:BA3)</f>
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D3" s="5">
         <f>IFERROR(D4/D2*D1,"")</f>
@@ -2068,7 +2065,7 @@
       </c>
       <c r="I3" s="5">
         <f>IFERROR(I4/I2*I1,"")</f>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="J3" s="5">
         <f>IFERROR(J4/J2*J1,"")</f>
@@ -2450,7 +2447,7 @@
       </c>
       <c r="B6" s="5">
         <f>IF(A6="","",SUM(D6:BA6))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="8" t="str">
         <f>IF(A6="","",SUMPRODUCT(D6:BA6,$D$4:$BA$4,1/IF($D$2:$BA$2&lt;&gt;"",$D$2:$BA$2,1)))</f>
@@ -2508,7 +2505,7 @@
         <v>0.0</v>
       </c>
       <c r="U6" s="9">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V6" s="9">
         <v>0.0</v>
@@ -2551,7 +2548,7 @@
       </c>
       <c r="B7" s="5">
         <f>IF(A7="","",SUM(D7:BA7))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7" s="8" t="str">
         <f>IF(A7="","",SUMPRODUCT(D7:BA7,$D$4:$BA$4,1/IF($D$2:$BA$2&lt;&gt;"",$D$2:$BA$2,1)))</f>
@@ -2573,7 +2570,7 @@
         <v>0.0</v>
       </c>
       <c r="I7" s="9">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J7" s="9">
         <v>0.0</v>
@@ -2609,7 +2606,7 @@
         <v>0.0</v>
       </c>
       <c r="U7" s="9">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="V7" s="9">
         <v>0.0</v>
@@ -6174,12 +6171,12 @@
   <dimension ref="A1:AMK130"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D2" sqref="D2:E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.388663967611" customWidth="true" style="1"/>
+    <col min="1" max="1" width="12.748987854251" customWidth="true" style="1"/>
     <col min="2" max="2" width="7.497975708502" customWidth="true" style="1"/>
     <col min="3" max="3" width="6.5344129554656" customWidth="true" style="1"/>
     <col min="4" max="4" width="8.1417004048583" customWidth="true" style="1"/>
@@ -7212,7 +7209,7 @@
       </c>
       <c r="B1" s="3">
         <f>SUM(D1:BA1)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="5">
@@ -7233,7 +7230,7 @@
       </c>
       <c r="H1" s="5">
         <f>IF(H5="","",SUM(H6:H81))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1" s="5">
         <f>IF(I5="","",SUM(I6:I81))</f>
@@ -7511,7 +7508,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="3">
         <f>SUM(D3:BA3)</f>
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5">
         <f>IFERROR(D4/D2*D1,"")</f>
@@ -7531,7 +7528,7 @@
       </c>
       <c r="H3" s="5">
         <f>IFERROR(H4/H2*H1,"")</f>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I3" s="5">
         <f>IFERROR(I4/I2*I1,"")</f>
@@ -7802,9 +7799,9 @@
       <c r="AZ4" s="5"/>
       <c r="BA4" s="5"/>
     </row>
-    <row r="5" spans="1:1025" customHeight="1" ht="13.8">
+    <row r="5" spans="1:1025" customHeight="1" ht="23.25">
       <c r="A5" s="5" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
@@ -7812,7 +7809,7 @@
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -7988,7 +7985,7 @@
       </c>
       <c r="B7" s="5">
         <f>IF(A7="","",SUM(D7:BA7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="8" t="str">
         <f>IF(A7="","",SUMPRODUCT(D7:BA7,$D$4:$BA$4,1/IF($D$2:$BA$2&lt;&gt;"",$D$2:$BA$2,1)))</f>
@@ -8007,7 +8004,7 @@
         <v>0.0</v>
       </c>
       <c r="H7" s="9">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I7" s="9">
         <v>0.0</v>
@@ -11657,12 +11654,12 @@
   <dimension ref="A1:AMK130"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D2" sqref="D2:E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.388663967611" customWidth="true" style="1"/>
+    <col min="1" max="1" width="12.63967611336" customWidth="true" style="1"/>
     <col min="2" max="2" width="7.497975708502" customWidth="true" style="1"/>
     <col min="3" max="3" width="6.5344129554656" customWidth="true" style="1"/>
     <col min="4" max="4" width="8.1417004048583" customWidth="true" style="1"/>
@@ -13241,9 +13238,9 @@
       <c r="AZ4" s="5"/>
       <c r="BA4" s="5"/>
     </row>
-    <row r="5" spans="1:1025" customHeight="1" ht="13.8">
+    <row r="5" spans="1:1025" customHeight="1" ht="23.25">
       <c r="A5" s="5" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
@@ -13251,7 +13248,7 @@
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -16216,7 +16213,7 @@
   <dimension ref="A1:AMK20"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2:E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17250,16 +17247,16 @@
   <sheetData>
     <row r="1" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>0</v>
@@ -17267,13 +17264,13 @@
     </row>
     <row r="2" spans="1:1025">
       <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -17284,13 +17281,13 @@
     </row>
     <row r="3" spans="1:1025">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
         <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>66</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -17301,13 +17298,13 @@
     </row>
     <row r="4" spans="1:1025">
       <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
         <v>67</v>
       </c>
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -17318,13 +17315,13 @@
     </row>
     <row r="5" spans="1:1025">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
         <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -17335,13 +17332,13 @@
     </row>
     <row r="6" spans="1:1025">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -17352,13 +17349,13 @@
     </row>
     <row r="7" spans="1:1025">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
         <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>66</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -17369,13 +17366,13 @@
     </row>
     <row r="8" spans="1:1025">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -17386,13 +17383,13 @@
     </row>
     <row r="9" spans="1:1025">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
         <v>65</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -17403,13 +17400,13 @@
     </row>
     <row r="10" spans="1:1025">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -17420,13 +17417,13 @@
     </row>
     <row r="11" spans="1:1025">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -17437,13 +17434,13 @@
     </row>
     <row r="12" spans="1:1025">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
         <v>65</v>
-      </c>
-      <c r="C12" t="s">
-        <v>66</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -17454,13 +17451,13 @@
     </row>
     <row r="13" spans="1:1025">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -17471,13 +17468,13 @@
     </row>
     <row r="14" spans="1:1025">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
         <v>65</v>
-      </c>
-      <c r="C14" t="s">
-        <v>66</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -17488,13 +17485,13 @@
     </row>
     <row r="15" spans="1:1025">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -17505,13 +17502,13 @@
     </row>
     <row r="16" spans="1:1025">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
         <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -17522,13 +17519,13 @@
     </row>
     <row r="17" spans="1:1025">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17">
         <v>4</v>
@@ -17539,13 +17536,13 @@
     </row>
     <row r="18" spans="1:1025">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
         <v>63</v>
-      </c>
-      <c r="C18" t="s">
-        <v>64</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -17556,13 +17553,13 @@
     </row>
     <row r="19" spans="1:1025">
       <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
         <v>77</v>
-      </c>
-      <c r="B19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" t="s">
-        <v>78</v>
       </c>
       <c r="D19">
         <v>6</v>
@@ -17573,13 +17570,13 @@
     </row>
     <row r="20" spans="1:1025">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D20">
         <v>6</v>

</xml_diff>

<commit_message>
pestanya inici, editar/esborrar assigns, arreglar bugs
</commit_message>
<xml_diff>
--- a/excel_emplenat.xlsx
+++ b/excel_emplenat.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
   <si>
     <t>Grups</t>
   </si>
@@ -53,18 +53,6 @@
     <t>ampli elect T</t>
   </si>
   <si>
-    <t>electronica P</t>
-  </si>
-  <si>
-    <t>electronica T</t>
-  </si>
-  <si>
-    <t>electrotecnia P</t>
-  </si>
-  <si>
-    <t>electrotecnia T</t>
-  </si>
-  <si>
     <t>fluids P</t>
   </si>
   <si>
@@ -86,25 +74,16 @@
     <t>sistemes T</t>
   </si>
   <si>
-    <t>taller elèctric T</t>
-  </si>
-  <si>
     <t>tallet elèctric P</t>
-  </si>
-  <si>
-    <t>tfg T</t>
-  </si>
-  <si>
-    <t>tfm T</t>
   </si>
   <si>
     <t>LB</t>
   </si>
   <si>
-    <t>JMME</t>
+    <t>MC</t>
   </si>
   <si>
-    <t>MC</t>
+    <t>JMME</t>
   </si>
   <si>
     <t>SB</t>
@@ -224,12 +203,6 @@
     <t>practica</t>
   </si>
   <si>
-    <t>electronica</t>
-  </si>
-  <si>
-    <t>electrotecnia</t>
-  </si>
-  <si>
     <t>fluids</t>
   </si>
   <si>
@@ -242,19 +215,7 @@
     <t>sistemes</t>
   </si>
   <si>
-    <t>taller elèctric</t>
-  </si>
-  <si>
     <t>tallet elèctric</t>
-  </si>
-  <si>
-    <t>tfg</t>
-  </si>
-  <si>
-    <t>tots</t>
-  </si>
-  <si>
-    <t>tfm</t>
   </si>
 </sst>
 </file>
@@ -1732,7 +1693,7 @@
       </c>
       <c r="B1" s="3">
         <f>SUM(D1:BA1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="5">
@@ -1781,35 +1742,35 @@
       </c>
       <c r="O1" s="5">
         <f>IF(O5="","",SUM(O6:O81))</f>
-        <v>0</v>
-      </c>
-      <c r="P1" s="5">
+        <v>4</v>
+      </c>
+      <c r="P1" s="5" t="str">
         <f>IF(P5="","",SUM(P6:P81))</f>
-        <v>0</v>
-      </c>
-      <c r="Q1" s="5">
+        <v/>
+      </c>
+      <c r="Q1" s="5" t="str">
         <f>IF(Q5="","",SUM(Q6:Q81))</f>
-        <v>4</v>
-      </c>
-      <c r="R1" s="5">
+        <v/>
+      </c>
+      <c r="R1" s="5" t="str">
         <f>IF(R5="","",SUM(R6:R81))</f>
-        <v>0</v>
-      </c>
-      <c r="S1" s="5">
+        <v/>
+      </c>
+      <c r="S1" s="5" t="str">
         <f>IF(S5="","",SUM(S6:S81))</f>
-        <v>0</v>
-      </c>
-      <c r="T1" s="5">
+        <v/>
+      </c>
+      <c r="T1" s="5" t="str">
         <f>IF(T5="","",SUM(T6:T81))</f>
-        <v>0</v>
-      </c>
-      <c r="U1" s="5">
+        <v/>
+      </c>
+      <c r="U1" s="5" t="str">
         <f>IF(U5="","",SUM(U6:U81))</f>
-        <v>1</v>
-      </c>
-      <c r="V1" s="5">
+        <v/>
+      </c>
+      <c r="V1" s="5" t="str">
         <f>IF(V5="","",SUM(V6:V81))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="W1" s="5" t="str">
         <f>IF(W5="","",SUM(W6:W81))</f>
@@ -1942,7 +1903,7 @@
       </c>
       <c r="B2" s="3">
         <f>SUM(D2:AMJ2)</f>
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5">
@@ -1958,50 +1919,36 @@
         <v>2</v>
       </c>
       <c r="H2" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I2" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K2" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L2" s="5">
         <v>3</v>
       </c>
       <c r="M2" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N2" s="5">
         <v>2</v>
       </c>
       <c r="O2" s="5">
-        <v>2</v>
-      </c>
-      <c r="P2" s="5">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="5">
         <v>4</v>
       </c>
-      <c r="R2" s="5">
-        <v>2</v>
-      </c>
-      <c r="S2" s="5">
-        <v>2</v>
-      </c>
-      <c r="T2" s="5">
-        <v>4</v>
-      </c>
-      <c r="U2" s="5">
-        <v>1</v>
-      </c>
-      <c r="V2" s="5">
-        <v>2</v>
-      </c>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
@@ -2041,7 +1988,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="3">
         <f>SUM(D3:BA3)</f>
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D3" s="5">
         <f>IFERROR(D4/D2*D1,"")</f>
@@ -2065,7 +2012,7 @@
       </c>
       <c r="I3" s="5">
         <f>IFERROR(I4/I2*I1,"")</f>
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="J3" s="5">
         <f>IFERROR(J4/J2*J1,"")</f>
@@ -2089,35 +2036,35 @@
       </c>
       <c r="O3" s="5">
         <f>IFERROR(O4/O2*O1,"")</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="5">
+        <v>36</v>
+      </c>
+      <c r="P3" s="5" t="str">
         <f>IFERROR(P4/P2*P1,"")</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="5">
+        <v/>
+      </c>
+      <c r="Q3" s="5" t="str">
         <f>IFERROR(Q4/Q2*Q1,"")</f>
-        <v>24</v>
-      </c>
-      <c r="R3" s="5">
+        <v/>
+      </c>
+      <c r="R3" s="5" t="str">
         <f>IFERROR(R4/R2*R1,"")</f>
-        <v>0</v>
-      </c>
-      <c r="S3" s="5">
+        <v/>
+      </c>
+      <c r="S3" s="5" t="str">
         <f>IFERROR(S4/S2*S1,"")</f>
-        <v>0</v>
-      </c>
-      <c r="T3" s="5">
+        <v/>
+      </c>
+      <c r="T3" s="5" t="str">
         <f>IFERROR(T4/T2*T1,"")</f>
-        <v>0</v>
-      </c>
-      <c r="U3" s="5">
+        <v/>
+      </c>
+      <c r="U3" s="5" t="str">
         <f>IFERROR(U4/U2*U1,"")</f>
-        <v>18</v>
-      </c>
-      <c r="V3" s="5">
+        <v/>
+      </c>
+      <c r="V3" s="5" t="str">
         <f>IFERROR(V4/V2*V1,"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="W3" s="5" t="str">
         <f>IFERROR(W4/W2*W1,"")</f>
@@ -2251,7 +2198,7 @@
       <c r="B4" s="4"/>
       <c r="C4" s="3">
         <f>SUM(D4:BA4)</f>
-        <v>420</v>
+        <v>261</v>
       </c>
       <c r="D4" s="5">
         <v>30</v>
@@ -2266,50 +2213,36 @@
         <v>12</v>
       </c>
       <c r="H4" s="5">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I4" s="5">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="J4" s="5">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="K4" s="5">
         <v>18</v>
       </c>
       <c r="L4" s="5">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="M4" s="5">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="N4" s="5">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="O4" s="5">
-        <v>18</v>
-      </c>
-      <c r="P4" s="5">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>24</v>
-      </c>
-      <c r="R4" s="5">
-        <v>24</v>
-      </c>
-      <c r="S4" s="5">
-        <v>24</v>
-      </c>
-      <c r="T4" s="5">
         <v>36</v>
       </c>
-      <c r="U4" s="5">
-        <v>18</v>
-      </c>
-      <c r="V4" s="5">
-        <v>36</v>
-      </c>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
@@ -2388,27 +2321,13 @@
       <c r="O5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
@@ -2443,11 +2362,11 @@
     </row>
     <row r="6" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5">
         <f>IF(A6="","",SUM(D6:BA6))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="8" t="str">
         <f>IF(A6="","",SUMPRODUCT(D6:BA6,$D$4:$BA$4,1/IF($D$2:$BA$2&lt;&gt;"",$D$2:$BA$2,1)))</f>
@@ -2487,29 +2406,19 @@
         <v>0.0</v>
       </c>
       <c r="O6" s="9">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="P6" s="9">
         <v>0.0</v>
       </c>
       <c r="Q6" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="R6" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S6" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T6" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U6" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="V6" s="9">
-        <v>0.0</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
       <c r="Y6" s="9"/>
@@ -2544,7 +2453,7 @@
     </row>
     <row r="7" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A7" s="5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5">
         <f>IF(A7="","",SUM(D7:BA7))</f>
@@ -2596,26 +2505,16 @@
       <c r="Q7" s="9">
         <v>0.0</v>
       </c>
-      <c r="R7" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S7" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T7" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U7" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V7" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
       <c r="W7" s="9"/>
     </row>
     <row r="8" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5">
         <f>IF(A8="","",SUM(D8:BA8))</f>
@@ -2667,26 +2566,16 @@
       <c r="Q8" s="9">
         <v>0.0</v>
       </c>
-      <c r="R8" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S8" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T8" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U8" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V8" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
       <c r="W8" s="9"/>
     </row>
     <row r="9" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A9" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5">
         <f>IF(A9="","",SUM(D9:BA9))</f>
@@ -2738,26 +2627,16 @@
       <c r="Q9" s="9">
         <v>0.0</v>
       </c>
-      <c r="R9" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S9" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T9" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U9" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V9" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
       <c r="W9" s="9"/>
     </row>
     <row r="10" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B10" s="5">
         <f>IF(A10="","",SUM(D10:BA10))</f>
@@ -2809,26 +2688,16 @@
       <c r="Q10" s="9">
         <v>0.0</v>
       </c>
-      <c r="R10" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S10" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T10" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U10" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V10" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
       <c r="W10" s="9"/>
     </row>
     <row r="11" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5">
         <f>IF(A11="","",SUM(D11:BA11))</f>
@@ -2880,26 +2749,16 @@
       <c r="Q11" s="9">
         <v>0.0</v>
       </c>
-      <c r="R11" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S11" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T11" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U11" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V11" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
       <c r="W11" s="9"/>
     </row>
     <row r="12" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5">
         <f>IF(A12="","",SUM(D12:BA12))</f>
@@ -2951,26 +2810,16 @@
       <c r="Q12" s="9">
         <v>0.0</v>
       </c>
-      <c r="R12" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S12" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T12" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U12" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V12" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
       <c r="W12" s="9"/>
     </row>
     <row r="13" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B13" s="5">
         <f>IF(A13="","",SUM(D13:BA13))</f>
@@ -3022,26 +2871,16 @@
       <c r="Q13" s="9">
         <v>0.0</v>
       </c>
-      <c r="R13" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S13" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T13" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U13" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V13" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
       <c r="W13" s="9"/>
     </row>
     <row r="14" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A14" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5">
         <f>IF(A14="","",SUM(D14:BA14))</f>
@@ -3093,26 +2932,16 @@
       <c r="Q14" s="9">
         <v>0.0</v>
       </c>
-      <c r="R14" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S14" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T14" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U14" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V14" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
       <c r="W14" s="9"/>
     </row>
     <row r="15" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A15" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5">
         <f>IF(A15="","",SUM(D15:BA15))</f>
@@ -3164,26 +2993,16 @@
       <c r="Q15" s="9">
         <v>0.0</v>
       </c>
-      <c r="R15" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S15" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T15" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U15" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V15" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
       <c r="W15" s="9"/>
     </row>
     <row r="16" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B16" s="5">
         <f>IF(A16="","",SUM(D16:BA16))</f>
@@ -3235,26 +3054,16 @@
       <c r="Q16" s="9">
         <v>0.0</v>
       </c>
-      <c r="R16" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S16" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T16" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U16" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V16" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
       <c r="W16" s="9"/>
     </row>
     <row r="17" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A17" s="5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B17" s="5">
         <f>IF(A17="","",SUM(D17:BA17))</f>
@@ -3306,26 +3115,16 @@
       <c r="Q17" s="9">
         <v>0.0</v>
       </c>
-      <c r="R17" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S17" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T17" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U17" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V17" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
       <c r="W17" s="9"/>
     </row>
     <row r="18" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A18" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5">
         <f>IF(A18="","",SUM(D18:BA18))</f>
@@ -3377,26 +3176,16 @@
       <c r="Q18" s="9">
         <v>0.0</v>
       </c>
-      <c r="R18" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S18" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T18" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U18" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V18" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
       <c r="W18" s="9"/>
     </row>
     <row r="19" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A19" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B19" s="5">
         <f>IF(A19="","",SUM(D19:BA19))</f>
@@ -3448,26 +3237,16 @@
       <c r="Q19" s="9">
         <v>0.0</v>
       </c>
-      <c r="R19" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S19" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T19" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U19" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V19" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
       <c r="W19" s="9"/>
     </row>
     <row r="20" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A20" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5">
         <f>IF(A20="","",SUM(D20:BA20))</f>
@@ -3519,26 +3298,16 @@
       <c r="Q20" s="9">
         <v>0.0</v>
       </c>
-      <c r="R20" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S20" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T20" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U20" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V20" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
       <c r="W20" s="9"/>
     </row>
     <row r="21" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A21" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B21" s="5">
         <f>IF(A21="","",SUM(D21:BA21))</f>
@@ -3590,26 +3359,16 @@
       <c r="Q21" s="9">
         <v>0.0</v>
       </c>
-      <c r="R21" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S21" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T21" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U21" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V21" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
       <c r="W21" s="9"/>
     </row>
     <row r="22" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A22" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B22" s="5">
         <f>IF(A22="","",SUM(D22:BA22))</f>
@@ -3661,26 +3420,16 @@
       <c r="Q22" s="9">
         <v>0.0</v>
       </c>
-      <c r="R22" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S22" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T22" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U22" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V22" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
       <c r="W22" s="9"/>
     </row>
     <row r="23" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A23" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5">
         <f>IF(A23="","",SUM(D23:BA23))</f>
@@ -3732,26 +3481,16 @@
       <c r="Q23" s="9">
         <v>0.0</v>
       </c>
-      <c r="R23" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S23" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T23" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U23" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V23" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
       <c r="W23" s="9"/>
     </row>
     <row r="24" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A24" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B24" s="5">
         <f>IF(A24="","",SUM(D24:BA24))</f>
@@ -3803,26 +3542,16 @@
       <c r="Q24" s="9">
         <v>0.0</v>
       </c>
-      <c r="R24" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S24" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T24" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U24" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V24" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
       <c r="W24" s="9"/>
     </row>
     <row r="25" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A25" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B25" s="5">
         <f>IF(A25="","",SUM(D25:BA25))</f>
@@ -3874,26 +3603,16 @@
       <c r="Q25" s="9">
         <v>0.0</v>
       </c>
-      <c r="R25" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S25" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T25" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U25" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V25" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
       <c r="W25" s="9"/>
     </row>
     <row r="26" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A26" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B26" s="5">
         <f>IF(A26="","",SUM(D26:BA26))</f>
@@ -3945,26 +3664,16 @@
       <c r="Q26" s="9">
         <v>0.0</v>
       </c>
-      <c r="R26" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S26" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T26" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U26" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V26" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
       <c r="W26" s="9"/>
     </row>
     <row r="27" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A27" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B27" s="5">
         <f>IF(A27="","",SUM(D27:BA27))</f>
@@ -4016,26 +3725,16 @@
       <c r="Q27" s="9">
         <v>0.0</v>
       </c>
-      <c r="R27" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S27" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T27" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U27" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V27" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
       <c r="W27" s="9"/>
     </row>
     <row r="28" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A28" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B28" s="5">
         <f>IF(A28="","",SUM(D28:BA28))</f>
@@ -4087,26 +3786,16 @@
       <c r="Q28" s="9">
         <v>0.0</v>
       </c>
-      <c r="R28" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S28" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T28" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U28" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V28" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
       <c r="W28" s="9"/>
     </row>
     <row r="29" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A29" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B29" s="5">
         <f>IF(A29="","",SUM(D29:BA29))</f>
@@ -4158,26 +3847,16 @@
       <c r="Q29" s="9">
         <v>0.0</v>
       </c>
-      <c r="R29" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S29" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T29" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U29" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V29" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
       <c r="W29" s="9"/>
     </row>
     <row r="30" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A30" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B30" s="5">
         <f>IF(A30="","",SUM(D30:BA30))</f>
@@ -4229,26 +3908,16 @@
       <c r="Q30" s="9">
         <v>0.0</v>
       </c>
-      <c r="R30" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S30" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T30" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U30" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V30" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
       <c r="W30" s="9"/>
     </row>
     <row r="31" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A31" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B31" s="5">
         <f>IF(A31="","",SUM(D31:BA31))</f>
@@ -4300,26 +3969,16 @@
       <c r="Q31" s="9">
         <v>0.0</v>
       </c>
-      <c r="R31" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S31" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T31" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U31" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V31" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
       <c r="W31" s="9"/>
     </row>
     <row r="32" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A32" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B32" s="5">
         <f>IF(A32="","",SUM(D32:BA32))</f>
@@ -4371,26 +4030,16 @@
       <c r="Q32" s="9">
         <v>0.0</v>
       </c>
-      <c r="R32" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S32" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T32" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U32" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V32" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
       <c r="W32" s="9"/>
     </row>
     <row r="33" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A33" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B33" s="5">
         <f>IF(A33="","",SUM(D33:BA33))</f>
@@ -4442,26 +4091,16 @@
       <c r="Q33" s="9">
         <v>0.0</v>
       </c>
-      <c r="R33" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S33" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T33" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U33" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V33" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
       <c r="W33" s="9"/>
     </row>
     <row r="34" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A34" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B34" s="5">
         <f>IF(A34="","",SUM(D34:BA34))</f>
@@ -4513,26 +4152,16 @@
       <c r="Q34" s="9">
         <v>0.0</v>
       </c>
-      <c r="R34" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S34" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T34" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U34" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V34" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="9"/>
+      <c r="U34" s="9"/>
+      <c r="V34" s="9"/>
       <c r="W34" s="9"/>
     </row>
     <row r="35" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A35" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B35" s="5">
         <f>IF(A35="","",SUM(D35:BA35))</f>
@@ -4584,26 +4213,16 @@
       <c r="Q35" s="9">
         <v>0.0</v>
       </c>
-      <c r="R35" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S35" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T35" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U35" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V35" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="9"/>
       <c r="W35" s="9"/>
     </row>
     <row r="36" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A36" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B36" s="5">
         <f>IF(A36="","",SUM(D36:BA36))</f>
@@ -4655,26 +4274,16 @@
       <c r="Q36" s="9">
         <v>0.0</v>
       </c>
-      <c r="R36" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S36" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T36" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U36" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V36" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="9"/>
+      <c r="V36" s="9"/>
       <c r="W36" s="9"/>
     </row>
     <row r="37" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A37" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B37" s="5">
         <f>IF(A37="","",SUM(D37:BA37))</f>
@@ -4726,26 +4335,16 @@
       <c r="Q37" s="9">
         <v>0.0</v>
       </c>
-      <c r="R37" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S37" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T37" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U37" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V37" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="9"/>
+      <c r="V37" s="9"/>
       <c r="W37" s="9"/>
     </row>
     <row r="38" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A38" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B38" s="5">
         <f>IF(A38="","",SUM(D38:BA38))</f>
@@ -4797,26 +4396,16 @@
       <c r="Q38" s="9">
         <v>0.0</v>
       </c>
-      <c r="R38" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S38" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T38" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U38" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V38" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
+      <c r="U38" s="9"/>
+      <c r="V38" s="9"/>
       <c r="W38" s="9"/>
     </row>
     <row r="39" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A39" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B39" s="5">
         <f>IF(A39="","",SUM(D39:BA39))</f>
@@ -4868,26 +4457,16 @@
       <c r="Q39" s="9">
         <v>0.0</v>
       </c>
-      <c r="R39" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S39" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T39" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U39" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V39" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="9"/>
       <c r="W39" s="9"/>
     </row>
     <row r="40" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A40" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B40" s="5">
         <f>IF(A40="","",SUM(D40:BA40))</f>
@@ -4939,26 +4518,16 @@
       <c r="Q40" s="9">
         <v>0.0</v>
       </c>
-      <c r="R40" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S40" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T40" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U40" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V40" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="9"/>
+      <c r="U40" s="9"/>
+      <c r="V40" s="9"/>
       <c r="W40" s="9"/>
     </row>
     <row r="41" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A41" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B41" s="5">
         <f>IF(A41="","",SUM(D41:BA41))</f>
@@ -5010,26 +4579,16 @@
       <c r="Q41" s="9">
         <v>0.0</v>
       </c>
-      <c r="R41" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S41" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T41" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U41" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V41" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R41" s="9"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="9"/>
+      <c r="U41" s="9"/>
+      <c r="V41" s="9"/>
       <c r="W41" s="9"/>
     </row>
     <row r="42" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A42" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B42" s="5">
         <f>IF(A42="","",SUM(D42:BA42))</f>
@@ -5081,26 +4640,16 @@
       <c r="Q42" s="9">
         <v>0.0</v>
       </c>
-      <c r="R42" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S42" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T42" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U42" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V42" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R42" s="9"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="9"/>
+      <c r="U42" s="9"/>
+      <c r="V42" s="9"/>
       <c r="W42" s="9"/>
     </row>
     <row r="43" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A43" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B43" s="5">
         <f>IF(A43="","",SUM(D43:BA43))</f>
@@ -5152,26 +4701,16 @@
       <c r="Q43" s="9">
         <v>0.0</v>
       </c>
-      <c r="R43" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S43" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T43" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U43" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V43" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R43" s="9"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="9"/>
+      <c r="U43" s="9"/>
+      <c r="V43" s="9"/>
       <c r="W43" s="9"/>
     </row>
     <row r="44" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A44" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B44" s="5">
         <f>IF(A44="","",SUM(D44:BA44))</f>
@@ -5223,21 +4762,11 @@
       <c r="Q44" s="9">
         <v>0.0</v>
       </c>
-      <c r="R44" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="S44" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="T44" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="U44" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="V44" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="R44" s="9"/>
+      <c r="S44" s="9"/>
+      <c r="T44" s="9"/>
+      <c r="U44" s="9"/>
+      <c r="V44" s="9"/>
       <c r="W44" s="9"/>
     </row>
     <row r="45" spans="1:1025" customHeight="1" ht="13.8">
@@ -7209,7 +6738,7 @@
       </c>
       <c r="B1" s="3">
         <f>SUM(D1:BA1)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="5">
@@ -7252,21 +6781,21 @@
         <f>IF(M5="","",SUM(M6:M81))</f>
         <v>0</v>
       </c>
-      <c r="N1" s="5">
+      <c r="N1" s="5" t="str">
         <f>IF(N5="","",SUM(N6:N81))</f>
-        <v>0</v>
-      </c>
-      <c r="O1" s="5">
+        <v/>
+      </c>
+      <c r="O1" s="5" t="str">
         <f>IF(O5="","",SUM(O6:O81))</f>
-        <v>0</v>
-      </c>
-      <c r="P1" s="5">
+        <v/>
+      </c>
+      <c r="P1" s="5" t="str">
         <f>IF(P5="","",SUM(P6:P81))</f>
-        <v>4</v>
-      </c>
-      <c r="Q1" s="5">
+        <v/>
+      </c>
+      <c r="Q1" s="5" t="str">
         <f>IF(Q5="","",SUM(Q6:Q81))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="R1" s="5" t="str">
         <f>IF(R5="","",SUM(R6:R81))</f>
@@ -7419,7 +6948,7 @@
       </c>
       <c r="B2" s="3">
         <f>SUM(D2:BA2)</f>
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5">
@@ -7432,38 +6961,30 @@
         <v>2</v>
       </c>
       <c r="G2" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H2" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I2" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K2" s="5">
         <v>3</v>
       </c>
       <c r="L2" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M2" s="5">
         <v>2</v>
       </c>
-      <c r="N2" s="5">
-        <v>2</v>
-      </c>
-      <c r="O2" s="5">
-        <v>3</v>
-      </c>
-      <c r="P2" s="5">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>2</v>
-      </c>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -7508,7 +7029,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="3">
         <f>SUM(D3:BA3)</f>
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="D3" s="5">
         <f>IFERROR(D4/D2*D1,"")</f>
@@ -7528,7 +7049,7 @@
       </c>
       <c r="H3" s="5">
         <f>IFERROR(H4/H2*H1,"")</f>
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="I3" s="5">
         <f>IFERROR(I4/I2*I1,"")</f>
@@ -7550,21 +7071,21 @@
         <f>IFERROR(M4/M2*M1,"")</f>
         <v>0</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="5" t="str">
         <f>IFERROR(N4/N2*N1,"")</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="5">
+        <v/>
+      </c>
+      <c r="O3" s="5" t="str">
         <f>IFERROR(O4/O2*O1,"")</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="5">
+        <v/>
+      </c>
+      <c r="P3" s="5" t="str">
         <f>IFERROR(P4/P2*P1,"")</f>
-        <v>24</v>
-      </c>
-      <c r="Q3" s="5">
+        <v/>
+      </c>
+      <c r="Q3" s="5" t="str">
         <f>IFERROR(Q4/Q2*Q1,"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="R3" s="5" t="str">
         <f>IFERROR(R4/R2*R1,"")</f>
@@ -7718,7 +7239,7 @@
       <c r="B4" s="4"/>
       <c r="C4" s="3">
         <f>SUM(D4:BA4)</f>
-        <v>276</v>
+        <v>195</v>
       </c>
       <c r="D4" s="5">
         <v>24</v>
@@ -7730,38 +7251,30 @@
         <v>12</v>
       </c>
       <c r="G4" s="5">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H4" s="5">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="I4" s="5">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="J4" s="5">
         <v>18</v>
       </c>
       <c r="K4" s="5">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="L4" s="5">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="M4" s="5">
-        <v>18</v>
-      </c>
-      <c r="N4" s="5">
-        <v>18</v>
-      </c>
-      <c r="O4" s="5">
-        <v>27</v>
-      </c>
-      <c r="P4" s="5">
         <v>24</v>
       </c>
-      <c r="Q4" s="5">
-        <v>24</v>
-      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -7839,18 +7352,10 @@
       <c r="M5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
@@ -7890,7 +7395,7 @@
     </row>
     <row r="6" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5">
         <f>IF(A6="","",SUM(D6:BA6))</f>
@@ -7931,17 +7436,13 @@
         <v>0.0</v>
       </c>
       <c r="N6" s="9">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="O6" s="9">
         <v>0.0</v>
       </c>
-      <c r="P6" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="Q6" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
@@ -7981,7 +7482,7 @@
     </row>
     <row r="7" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A7" s="5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5">
         <f>IF(A7="","",SUM(D7:BA7))</f>
@@ -8027,12 +7528,8 @@
       <c r="O7" s="9">
         <v>0.0</v>
       </c>
-      <c r="P7" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q7" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
@@ -8042,7 +7539,7 @@
     </row>
     <row r="8" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5">
         <f>IF(A8="","",SUM(D8:BA8))</f>
@@ -8088,12 +7585,8 @@
       <c r="O8" s="9">
         <v>0.0</v>
       </c>
-      <c r="P8" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q8" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
       <c r="T8" s="9"/>
@@ -8103,7 +7596,7 @@
     </row>
     <row r="9" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A9" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5">
         <f>IF(A9="","",SUM(D9:BA9))</f>
@@ -8149,12 +7642,8 @@
       <c r="O9" s="9">
         <v>0.0</v>
       </c>
-      <c r="P9" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q9" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
       <c r="T9" s="9"/>
@@ -8164,7 +7653,7 @@
     </row>
     <row r="10" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B10" s="5">
         <f>IF(A10="","",SUM(D10:BA10))</f>
@@ -8210,12 +7699,8 @@
       <c r="O10" s="9">
         <v>0.0</v>
       </c>
-      <c r="P10" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q10" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
       <c r="T10" s="9"/>
@@ -8225,7 +7710,7 @@
     </row>
     <row r="11" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5">
         <f>IF(A11="","",SUM(D11:BA11))</f>
@@ -8271,12 +7756,8 @@
       <c r="O11" s="9">
         <v>0.0</v>
       </c>
-      <c r="P11" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q11" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
       <c r="T11" s="9"/>
@@ -8286,7 +7767,7 @@
     </row>
     <row r="12" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5">
         <f>IF(A12="","",SUM(D12:BA12))</f>
@@ -8332,12 +7813,8 @@
       <c r="O12" s="9">
         <v>0.0</v>
       </c>
-      <c r="P12" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q12" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
       <c r="R12" s="9"/>
       <c r="S12" s="9"/>
       <c r="T12" s="9"/>
@@ -8347,7 +7824,7 @@
     </row>
     <row r="13" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B13" s="5">
         <f>IF(A13="","",SUM(D13:BA13))</f>
@@ -8393,12 +7870,8 @@
       <c r="O13" s="9">
         <v>0.0</v>
       </c>
-      <c r="P13" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q13" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
       <c r="R13" s="9"/>
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
@@ -8408,7 +7881,7 @@
     </row>
     <row r="14" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A14" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5">
         <f>IF(A14="","",SUM(D14:BA14))</f>
@@ -8454,12 +7927,8 @@
       <c r="O14" s="9">
         <v>0.0</v>
       </c>
-      <c r="P14" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q14" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
       <c r="S14" s="9"/>
       <c r="T14" s="9"/>
@@ -8469,7 +7938,7 @@
     </row>
     <row r="15" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A15" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5">
         <f>IF(A15="","",SUM(D15:BA15))</f>
@@ -8515,12 +7984,8 @@
       <c r="O15" s="9">
         <v>0.0</v>
       </c>
-      <c r="P15" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q15" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
       <c r="T15" s="9"/>
@@ -8530,7 +7995,7 @@
     </row>
     <row r="16" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B16" s="5">
         <f>IF(A16="","",SUM(D16:BA16))</f>
@@ -8576,12 +8041,8 @@
       <c r="O16" s="9">
         <v>0.0</v>
       </c>
-      <c r="P16" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q16" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
       <c r="T16" s="9"/>
@@ -8591,7 +8052,7 @@
     </row>
     <row r="17" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A17" s="5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B17" s="5">
         <f>IF(A17="","",SUM(D17:BA17))</f>
@@ -8637,12 +8098,8 @@
       <c r="O17" s="9">
         <v>0.0</v>
       </c>
-      <c r="P17" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q17" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
@@ -8652,7 +8109,7 @@
     </row>
     <row r="18" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A18" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5">
         <f>IF(A18="","",SUM(D18:BA18))</f>
@@ -8698,12 +8155,8 @@
       <c r="O18" s="9">
         <v>0.0</v>
       </c>
-      <c r="P18" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q18" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
       <c r="T18" s="9"/>
@@ -8713,7 +8166,7 @@
     </row>
     <row r="19" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A19" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B19" s="5">
         <f>IF(A19="","",SUM(D19:BA19))</f>
@@ -8759,12 +8212,8 @@
       <c r="O19" s="9">
         <v>0.0</v>
       </c>
-      <c r="P19" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q19" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
       <c r="T19" s="9"/>
@@ -8774,7 +8223,7 @@
     </row>
     <row r="20" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A20" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5">
         <f>IF(A20="","",SUM(D20:BA20))</f>
@@ -8820,12 +8269,8 @@
       <c r="O20" s="9">
         <v>0.0</v>
       </c>
-      <c r="P20" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q20" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
@@ -8835,7 +8280,7 @@
     </row>
     <row r="21" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A21" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B21" s="5">
         <f>IF(A21="","",SUM(D21:BA21))</f>
@@ -8881,12 +8326,8 @@
       <c r="O21" s="9">
         <v>0.0</v>
       </c>
-      <c r="P21" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q21" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
@@ -8896,7 +8337,7 @@
     </row>
     <row r="22" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A22" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B22" s="5">
         <f>IF(A22="","",SUM(D22:BA22))</f>
@@ -8942,12 +8383,8 @@
       <c r="O22" s="9">
         <v>0.0</v>
       </c>
-      <c r="P22" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q22" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
@@ -8957,7 +8394,7 @@
     </row>
     <row r="23" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A23" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5">
         <f>IF(A23="","",SUM(D23:BA23))</f>
@@ -9003,12 +8440,8 @@
       <c r="O23" s="9">
         <v>0.0</v>
       </c>
-      <c r="P23" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q23" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
       <c r="T23" s="9"/>
@@ -9018,7 +8451,7 @@
     </row>
     <row r="24" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A24" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B24" s="5">
         <f>IF(A24="","",SUM(D24:BA24))</f>
@@ -9064,12 +8497,8 @@
       <c r="O24" s="9">
         <v>0.0</v>
       </c>
-      <c r="P24" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q24" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
@@ -9079,7 +8508,7 @@
     </row>
     <row r="25" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A25" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B25" s="5">
         <f>IF(A25="","",SUM(D25:BA25))</f>
@@ -9125,12 +8554,8 @@
       <c r="O25" s="9">
         <v>0.0</v>
       </c>
-      <c r="P25" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q25" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
@@ -9140,7 +8565,7 @@
     </row>
     <row r="26" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A26" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B26" s="5">
         <f>IF(A26="","",SUM(D26:BA26))</f>
@@ -9186,12 +8611,8 @@
       <c r="O26" s="9">
         <v>0.0</v>
       </c>
-      <c r="P26" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q26" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
       <c r="T26" s="9"/>
@@ -9201,7 +8622,7 @@
     </row>
     <row r="27" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A27" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B27" s="5">
         <f>IF(A27="","",SUM(D27:BA27))</f>
@@ -9247,12 +8668,8 @@
       <c r="O27" s="9">
         <v>0.0</v>
       </c>
-      <c r="P27" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q27" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
@@ -9262,7 +8679,7 @@
     </row>
     <row r="28" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A28" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B28" s="5">
         <f>IF(A28="","",SUM(D28:BA28))</f>
@@ -9308,12 +8725,8 @@
       <c r="O28" s="9">
         <v>0.0</v>
       </c>
-      <c r="P28" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q28" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
       <c r="T28" s="9"/>
@@ -9323,7 +8736,7 @@
     </row>
     <row r="29" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A29" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B29" s="5">
         <f>IF(A29="","",SUM(D29:BA29))</f>
@@ -9369,12 +8782,8 @@
       <c r="O29" s="9">
         <v>0.0</v>
       </c>
-      <c r="P29" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q29" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
       <c r="T29" s="9"/>
@@ -9384,7 +8793,7 @@
     </row>
     <row r="30" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A30" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B30" s="5">
         <f>IF(A30="","",SUM(D30:BA30))</f>
@@ -9430,12 +8839,8 @@
       <c r="O30" s="9">
         <v>0.0</v>
       </c>
-      <c r="P30" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q30" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
       <c r="T30" s="9"/>
@@ -9445,7 +8850,7 @@
     </row>
     <row r="31" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A31" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B31" s="5">
         <f>IF(A31="","",SUM(D31:BA31))</f>
@@ -9491,12 +8896,8 @@
       <c r="O31" s="9">
         <v>0.0</v>
       </c>
-      <c r="P31" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q31" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
@@ -9506,7 +8907,7 @@
     </row>
     <row r="32" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A32" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B32" s="5">
         <f>IF(A32="","",SUM(D32:BA32))</f>
@@ -9552,12 +8953,8 @@
       <c r="O32" s="9">
         <v>0.0</v>
       </c>
-      <c r="P32" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q32" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
       <c r="T32" s="9"/>
@@ -9567,7 +8964,7 @@
     </row>
     <row r="33" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A33" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B33" s="5">
         <f>IF(A33="","",SUM(D33:BA33))</f>
@@ -9613,12 +9010,8 @@
       <c r="O33" s="9">
         <v>0.0</v>
       </c>
-      <c r="P33" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q33" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
       <c r="T33" s="9"/>
@@ -9628,7 +9021,7 @@
     </row>
     <row r="34" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A34" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B34" s="5">
         <f>IF(A34="","",SUM(D34:BA34))</f>
@@ -9674,12 +9067,8 @@
       <c r="O34" s="9">
         <v>0.0</v>
       </c>
-      <c r="P34" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q34" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
       <c r="R34" s="9"/>
       <c r="S34" s="9"/>
       <c r="T34" s="9"/>
@@ -9689,7 +9078,7 @@
     </row>
     <row r="35" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A35" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B35" s="5">
         <f>IF(A35="","",SUM(D35:BA35))</f>
@@ -9735,12 +9124,8 @@
       <c r="O35" s="9">
         <v>0.0</v>
       </c>
-      <c r="P35" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q35" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
       <c r="R35" s="9"/>
       <c r="S35" s="9"/>
       <c r="T35" s="9"/>
@@ -9750,7 +9135,7 @@
     </row>
     <row r="36" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A36" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B36" s="5">
         <f>IF(A36="","",SUM(D36:BA36))</f>
@@ -9796,12 +9181,8 @@
       <c r="O36" s="9">
         <v>0.0</v>
       </c>
-      <c r="P36" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q36" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
       <c r="R36" s="9"/>
       <c r="S36" s="9"/>
       <c r="T36" s="9"/>
@@ -9811,7 +9192,7 @@
     </row>
     <row r="37" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A37" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B37" s="5">
         <f>IF(A37="","",SUM(D37:BA37))</f>
@@ -9857,12 +9238,8 @@
       <c r="O37" s="9">
         <v>0.0</v>
       </c>
-      <c r="P37" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q37" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
       <c r="R37" s="9"/>
       <c r="S37" s="9"/>
       <c r="T37" s="9"/>
@@ -9872,7 +9249,7 @@
     </row>
     <row r="38" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A38" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B38" s="5">
         <f>IF(A38="","",SUM(D38:BA38))</f>
@@ -9918,12 +9295,8 @@
       <c r="O38" s="9">
         <v>0.0</v>
       </c>
-      <c r="P38" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q38" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
       <c r="R38" s="9"/>
       <c r="S38" s="9"/>
       <c r="T38" s="9"/>
@@ -9933,7 +9306,7 @@
     </row>
     <row r="39" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A39" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B39" s="5">
         <f>IF(A39="","",SUM(D39:BA39))</f>
@@ -9979,12 +9352,8 @@
       <c r="O39" s="9">
         <v>0.0</v>
       </c>
-      <c r="P39" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q39" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
       <c r="R39" s="9"/>
       <c r="S39" s="9"/>
       <c r="T39" s="9"/>
@@ -9994,7 +9363,7 @@
     </row>
     <row r="40" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A40" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B40" s="5">
         <f>IF(A40="","",SUM(D40:BA40))</f>
@@ -10040,12 +9409,8 @@
       <c r="O40" s="9">
         <v>0.0</v>
       </c>
-      <c r="P40" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q40" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
       <c r="R40" s="9"/>
       <c r="S40" s="9"/>
       <c r="T40" s="9"/>
@@ -10055,7 +9420,7 @@
     </row>
     <row r="41" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A41" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B41" s="5">
         <f>IF(A41="","",SUM(D41:BA41))</f>
@@ -10101,12 +9466,8 @@
       <c r="O41" s="9">
         <v>0.0</v>
       </c>
-      <c r="P41" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q41" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
       <c r="R41" s="9"/>
       <c r="S41" s="9"/>
       <c r="T41" s="9"/>
@@ -10116,7 +9477,7 @@
     </row>
     <row r="42" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A42" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B42" s="5">
         <f>IF(A42="","",SUM(D42:BA42))</f>
@@ -10162,12 +9523,8 @@
       <c r="O42" s="9">
         <v>0.0</v>
       </c>
-      <c r="P42" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q42" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
       <c r="R42" s="9"/>
       <c r="S42" s="9"/>
       <c r="T42" s="9"/>
@@ -10177,7 +9534,7 @@
     </row>
     <row r="43" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A43" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B43" s="5">
         <f>IF(A43="","",SUM(D43:BA43))</f>
@@ -10223,12 +9580,8 @@
       <c r="O43" s="9">
         <v>0.0</v>
       </c>
-      <c r="P43" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q43" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
       <c r="R43" s="9"/>
       <c r="S43" s="9"/>
       <c r="T43" s="9"/>
@@ -10238,7 +9591,7 @@
     </row>
     <row r="44" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A44" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B44" s="5">
         <f>IF(A44="","",SUM(D44:BA44))</f>
@@ -10284,12 +9637,8 @@
       <c r="O44" s="9">
         <v>0.0</v>
       </c>
-      <c r="P44" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="Q44" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
       <c r="R44" s="9"/>
       <c r="S44" s="9"/>
       <c r="T44" s="9"/>
@@ -12703,9 +12052,9 @@
         <f>IF(E5="","",SUM(E6:E81))</f>
         <v>0</v>
       </c>
-      <c r="F1" s="5">
+      <c r="F1" s="5" t="str">
         <f>IF(F5="","",SUM(F6:F81))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="G1" s="5" t="str">
         <f>IF(G5="","",SUM(G6:G81))</f>
@@ -12902,18 +12251,16 @@
       </c>
       <c r="B2" s="3">
         <f>SUM(D2:BA2)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5">
         <v>2</v>
       </c>
       <c r="E2" s="5">
-        <v>2</v>
-      </c>
-      <c r="F2" s="5">
         <v>4</v>
       </c>
+      <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -12979,9 +12326,9 @@
         <f>IFERROR(E4/E2*E1,"")</f>
         <v>0</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="5" t="str">
         <f>IFERROR(F4/F2*F1,"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="G3" s="5" t="str">
         <f>IFERROR(G4/G2*G1,"")</f>
@@ -13179,17 +12526,15 @@
       <c r="B4" s="4"/>
       <c r="C4" s="3">
         <f>SUM(D4:BA4)</f>
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="D4" s="5">
         <v>30</v>
       </c>
       <c r="E4" s="5">
-        <v>24</v>
-      </c>
-      <c r="F4" s="5">
         <v>36</v>
       </c>
+      <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -13252,11 +12597,9 @@
         <v>7</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -13307,7 +12650,7 @@
     </row>
     <row r="6" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5">
         <f>IF(A6="","",SUM(D6:BA6))</f>
@@ -13323,9 +12666,7 @@
       <c r="E6" s="9">
         <v>0.0</v>
       </c>
-      <c r="F6" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -13376,7 +12717,7 @@
     </row>
     <row r="7" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A7" s="5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5">
         <f>IF(A7="","",SUM(D7:BA7))</f>
@@ -13392,9 +12733,7 @@
       <c r="E7" s="9">
         <v>0.0</v>
       </c>
-      <c r="F7" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -13415,7 +12754,7 @@
     </row>
     <row r="8" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5">
         <f>IF(A8="","",SUM(D8:BA8))</f>
@@ -13431,9 +12770,7 @@
       <c r="E8" s="9">
         <v>0.0</v>
       </c>
-      <c r="F8" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -13454,7 +12791,7 @@
     </row>
     <row r="9" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A9" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5">
         <f>IF(A9="","",SUM(D9:BA9))</f>
@@ -13470,9 +12807,7 @@
       <c r="E9" s="9">
         <v>0.0</v>
       </c>
-      <c r="F9" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -13493,7 +12828,7 @@
     </row>
     <row r="10" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B10" s="5">
         <f>IF(A10="","",SUM(D10:BA10))</f>
@@ -13509,9 +12844,7 @@
       <c r="E10" s="9">
         <v>0.0</v>
       </c>
-      <c r="F10" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -13532,7 +12865,7 @@
     </row>
     <row r="11" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5">
         <f>IF(A11="","",SUM(D11:BA11))</f>
@@ -13548,9 +12881,7 @@
       <c r="E11" s="9">
         <v>0.0</v>
       </c>
-      <c r="F11" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -13571,7 +12902,7 @@
     </row>
     <row r="12" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5">
         <f>IF(A12="","",SUM(D12:BA12))</f>
@@ -13587,9 +12918,7 @@
       <c r="E12" s="9">
         <v>0.0</v>
       </c>
-      <c r="F12" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
@@ -13610,7 +12939,7 @@
     </row>
     <row r="13" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B13" s="5">
         <f>IF(A13="","",SUM(D13:BA13))</f>
@@ -13626,9 +12955,7 @@
       <c r="E13" s="9">
         <v>0.0</v>
       </c>
-      <c r="F13" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -13649,7 +12976,7 @@
     </row>
     <row r="14" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A14" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5">
         <f>IF(A14="","",SUM(D14:BA14))</f>
@@ -13665,9 +12992,7 @@
       <c r="E14" s="9">
         <v>0.0</v>
       </c>
-      <c r="F14" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -13688,7 +13013,7 @@
     </row>
     <row r="15" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A15" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5">
         <f>IF(A15="","",SUM(D15:BA15))</f>
@@ -13704,9 +13029,7 @@
       <c r="E15" s="9">
         <v>0.0</v>
       </c>
-      <c r="F15" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -13727,7 +13050,7 @@
     </row>
     <row r="16" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B16" s="5">
         <f>IF(A16="","",SUM(D16:BA16))</f>
@@ -13743,9 +13066,7 @@
       <c r="E16" s="9">
         <v>0.0</v>
       </c>
-      <c r="F16" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -13766,7 +13087,7 @@
     </row>
     <row r="17" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A17" s="5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B17" s="5">
         <f>IF(A17="","",SUM(D17:BA17))</f>
@@ -13782,9 +13103,7 @@
       <c r="E17" s="9">
         <v>0.0</v>
       </c>
-      <c r="F17" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -13805,7 +13124,7 @@
     </row>
     <row r="18" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A18" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5">
         <f>IF(A18="","",SUM(D18:BA18))</f>
@@ -13821,9 +13140,7 @@
       <c r="E18" s="9">
         <v>0.0</v>
       </c>
-      <c r="F18" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -13844,7 +13161,7 @@
     </row>
     <row r="19" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A19" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B19" s="5">
         <f>IF(A19="","",SUM(D19:BA19))</f>
@@ -13860,9 +13177,7 @@
       <c r="E19" s="9">
         <v>0.0</v>
       </c>
-      <c r="F19" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -13883,7 +13198,7 @@
     </row>
     <row r="20" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A20" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5">
         <f>IF(A20="","",SUM(D20:BA20))</f>
@@ -13899,9 +13214,7 @@
       <c r="E20" s="9">
         <v>0.0</v>
       </c>
-      <c r="F20" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -13922,7 +13235,7 @@
     </row>
     <row r="21" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A21" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B21" s="5">
         <f>IF(A21="","",SUM(D21:BA21))</f>
@@ -13938,9 +13251,7 @@
       <c r="E21" s="9">
         <v>0.0</v>
       </c>
-      <c r="F21" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -13961,7 +13272,7 @@
     </row>
     <row r="22" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A22" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B22" s="5">
         <f>IF(A22="","",SUM(D22:BA22))</f>
@@ -13977,9 +13288,7 @@
       <c r="E22" s="9">
         <v>0.0</v>
       </c>
-      <c r="F22" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -14000,7 +13309,7 @@
     </row>
     <row r="23" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A23" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5">
         <f>IF(A23="","",SUM(D23:BA23))</f>
@@ -14016,9 +13325,7 @@
       <c r="E23" s="9">
         <v>0.0</v>
       </c>
-      <c r="F23" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
@@ -14039,7 +13346,7 @@
     </row>
     <row r="24" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A24" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B24" s="5">
         <f>IF(A24="","",SUM(D24:BA24))</f>
@@ -14055,9 +13362,7 @@
       <c r="E24" s="9">
         <v>0.0</v>
       </c>
-      <c r="F24" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
@@ -14078,7 +13383,7 @@
     </row>
     <row r="25" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A25" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B25" s="5">
         <f>IF(A25="","",SUM(D25:BA25))</f>
@@ -14094,9 +13399,7 @@
       <c r="E25" s="9">
         <v>0.0</v>
       </c>
-      <c r="F25" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
@@ -14117,7 +13420,7 @@
     </row>
     <row r="26" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A26" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B26" s="5">
         <f>IF(A26="","",SUM(D26:BA26))</f>
@@ -14133,9 +13436,7 @@
       <c r="E26" s="9">
         <v>0.0</v>
       </c>
-      <c r="F26" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -14156,7 +13457,7 @@
     </row>
     <row r="27" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A27" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B27" s="5">
         <f>IF(A27="","",SUM(D27:BA27))</f>
@@ -14172,9 +13473,7 @@
       <c r="E27" s="9">
         <v>0.0</v>
       </c>
-      <c r="F27" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -14195,7 +13494,7 @@
     </row>
     <row r="28" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A28" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B28" s="5">
         <f>IF(A28="","",SUM(D28:BA28))</f>
@@ -14211,9 +13510,7 @@
       <c r="E28" s="9">
         <v>0.0</v>
       </c>
-      <c r="F28" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
@@ -14234,7 +13531,7 @@
     </row>
     <row r="29" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A29" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B29" s="5">
         <f>IF(A29="","",SUM(D29:BA29))</f>
@@ -14250,9 +13547,7 @@
       <c r="E29" s="9">
         <v>0.0</v>
       </c>
-      <c r="F29" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
@@ -14273,7 +13568,7 @@
     </row>
     <row r="30" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A30" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B30" s="5">
         <f>IF(A30="","",SUM(D30:BA30))</f>
@@ -14289,9 +13584,7 @@
       <c r="E30" s="9">
         <v>0.0</v>
       </c>
-      <c r="F30" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -14312,7 +13605,7 @@
     </row>
     <row r="31" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A31" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B31" s="5">
         <f>IF(A31="","",SUM(D31:BA31))</f>
@@ -14328,9 +13621,7 @@
       <c r="E31" s="9">
         <v>0.0</v>
       </c>
-      <c r="F31" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
@@ -14351,7 +13642,7 @@
     </row>
     <row r="32" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A32" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B32" s="5">
         <f>IF(A32="","",SUM(D32:BA32))</f>
@@ -14367,9 +13658,7 @@
       <c r="E32" s="9">
         <v>0.0</v>
       </c>
-      <c r="F32" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -14390,7 +13679,7 @@
     </row>
     <row r="33" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A33" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B33" s="5">
         <f>IF(A33="","",SUM(D33:BA33))</f>
@@ -14406,9 +13695,7 @@
       <c r="E33" s="9">
         <v>0.0</v>
       </c>
-      <c r="F33" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -14429,7 +13716,7 @@
     </row>
     <row r="34" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A34" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B34" s="5">
         <f>IF(A34="","",SUM(D34:BA34))</f>
@@ -14445,9 +13732,7 @@
       <c r="E34" s="9">
         <v>0.0</v>
       </c>
-      <c r="F34" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -14468,7 +13753,7 @@
     </row>
     <row r="35" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A35" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B35" s="5">
         <f>IF(A35="","",SUM(D35:BA35))</f>
@@ -14484,9 +13769,7 @@
       <c r="E35" s="9">
         <v>0.0</v>
       </c>
-      <c r="F35" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
@@ -14507,7 +13790,7 @@
     </row>
     <row r="36" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A36" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B36" s="5">
         <f>IF(A36="","",SUM(D36:BA36))</f>
@@ -14523,9 +13806,7 @@
       <c r="E36" s="9">
         <v>0.0</v>
       </c>
-      <c r="F36" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
@@ -14546,7 +13827,7 @@
     </row>
     <row r="37" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A37" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B37" s="5">
         <f>IF(A37="","",SUM(D37:BA37))</f>
@@ -14562,9 +13843,7 @@
       <c r="E37" s="9">
         <v>0.0</v>
       </c>
-      <c r="F37" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
@@ -14585,7 +13864,7 @@
     </row>
     <row r="38" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A38" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B38" s="5">
         <f>IF(A38="","",SUM(D38:BA38))</f>
@@ -14601,9 +13880,7 @@
       <c r="E38" s="9">
         <v>0.0</v>
       </c>
-      <c r="F38" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F38" s="9"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
@@ -14624,7 +13901,7 @@
     </row>
     <row r="39" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A39" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B39" s="5">
         <f>IF(A39="","",SUM(D39:BA39))</f>
@@ -14640,9 +13917,7 @@
       <c r="E39" s="9">
         <v>0.0</v>
       </c>
-      <c r="F39" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F39" s="9"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -14663,7 +13938,7 @@
     </row>
     <row r="40" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A40" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B40" s="5">
         <f>IF(A40="","",SUM(D40:BA40))</f>
@@ -14679,9 +13954,7 @@
       <c r="E40" s="9">
         <v>0.0</v>
       </c>
-      <c r="F40" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
@@ -14702,7 +13975,7 @@
     </row>
     <row r="41" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A41" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B41" s="5">
         <f>IF(A41="","",SUM(D41:BA41))</f>
@@ -14718,9 +13991,7 @@
       <c r="E41" s="9">
         <v>0.0</v>
       </c>
-      <c r="F41" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -14741,7 +14012,7 @@
     </row>
     <row r="42" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A42" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B42" s="5">
         <f>IF(A42="","",SUM(D42:BA42))</f>
@@ -14757,9 +14028,7 @@
       <c r="E42" s="9">
         <v>0.0</v>
       </c>
-      <c r="F42" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
@@ -14780,7 +14049,7 @@
     </row>
     <row r="43" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A43" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B43" s="5">
         <f>IF(A43="","",SUM(D43:BA43))</f>
@@ -14796,9 +14065,7 @@
       <c r="E43" s="9">
         <v>0.0</v>
       </c>
-      <c r="F43" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
@@ -14819,7 +14086,7 @@
     </row>
     <row r="44" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A44" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B44" s="5">
         <f>IF(A44="","",SUM(D44:BA44))</f>
@@ -14835,9 +14102,7 @@
       <c r="E44" s="9">
         <v>0.0</v>
       </c>
-      <c r="F44" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
@@ -16210,7 +15475,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AMK20"/>
+  <dimension ref="A1:AMK13"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="D2" sqref="D2:E174"/>
@@ -17247,16 +16512,16 @@
   <sheetData>
     <row r="1" spans="1:1025" customHeight="1" ht="13.8">
       <c r="A1" s="10" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>0</v>
@@ -17264,13 +16529,13 @@
     </row>
     <row r="2" spans="1:1025">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -17281,13 +16546,13 @@
     </row>
     <row r="3" spans="1:1025">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -17298,13 +16563,13 @@
     </row>
     <row r="4" spans="1:1025">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -17315,13 +16580,13 @@
     </row>
     <row r="5" spans="1:1025">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -17332,84 +16597,84 @@
     </row>
     <row r="6" spans="1:1025">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
         <v>3</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:1025">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1025">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:1025">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
         <v>2</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:1025">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -17417,33 +16682,33 @@
     </row>
     <row r="11" spans="1:1025">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:1025">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -17451,138 +16716,19 @@
     </row>
     <row r="13" spans="1:1025">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1025">
-      <c r="A14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1025">
-      <c r="A15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
         <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1025">
-      <c r="A16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1025">
-      <c r="A17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17">
-        <v>4</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1025">
-      <c r="A18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="E18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1025">
-      <c r="A19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19">
-        <v>6</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1025">
-      <c r="A20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20">
-        <v>6</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
boto tirar enrere, pressupost, editar admin
</commit_message>
<xml_diff>
--- a/excel_emplenat.xlsx
+++ b/excel_emplenat.xlsx
@@ -1568,12 +1568,12 @@
       </c>
       <c r="B1" s="3">
         <f>SUM(D1:BA1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="5">
         <f>IF(D5="","",SUM(D6:D81))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="5">
         <f>IF(E5="","",SUM(E6:E81))</f>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="F1" s="5">
         <f>IF(F5="","",SUM(F6:F81))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1" s="5" t="str">
         <f>IF(G5="","",SUM(G6:G81))</f>
@@ -1845,11 +1845,11 @@
       <c r="B3" s="4"/>
       <c r="C3" s="3">
         <f>SUM(D3:BA3)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D3" s="5">
         <f>IFERROR(D4/D2*D1,"")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E3" s="5">
         <f>IFERROR(E4/E2*E1,"")</f>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="F3" s="5">
         <f>IFERROR(F4/F2*F1,"")</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G3" s="5" t="str">
         <f>IFERROR(G4/G2*G1,"")</f>
@@ -2187,20 +2187,20 @@
       </c>
       <c r="B6" s="5">
         <f>IF(A6="","",SUM(D6:BA6))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="8">
         <f>IF(A6="","",SUMPRODUCT(D6:BA6,$D$83:$BA$83))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D6" s="9">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" s="9">
         <v>0.0</v>
       </c>
       <c r="F6" s="9">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -5792,12 +5792,12 @@
       </c>
       <c r="B1" s="3">
         <f>SUM(D1:BA1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="5">
         <f>IF(D5="","",SUM(D6:D81))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="5" t="str">
         <f>IF(E5="","",SUM(E6:E81))</f>
@@ -6065,11 +6065,11 @@
       <c r="B3" s="4"/>
       <c r="C3" s="3">
         <f>SUM(D3:BA3)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D3" s="5">
         <f>IFERROR(D4/D2*D1,"")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E3" s="5" t="str">
         <f>IFERROR(E4/E2*E1,"")</f>
@@ -6399,14 +6399,14 @@
       </c>
       <c r="B6" s="5">
         <f>IF(A6="","",SUM(D6:BA6))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="8">
         <f>IF(A6="","",SUMPRODUCT(D6:BA6,D83:BA83))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D6" s="9">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>

</xml_diff>